<commit_message>
added remove group operation
</commit_message>
<xml_diff>
--- a/IOUsing/data/UniversityContents.xlsx
+++ b/IOUsing/data/UniversityContents.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="29">
   <si>
     <t>Full Name</t>
   </si>
@@ -574,7 +574,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -692,34 +692,12 @@
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B11" t="n" s="0">
-        <v>11.0</v>
+        <v>13.0</v>
       </c>
       <c r="C11" t="n" s="0">
-        <v>321.0</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s" s="0">
-        <v>26</v>
-      </c>
-      <c r="B12" t="n" s="0">
-        <v>12.0</v>
-      </c>
-      <c r="C12" t="n" s="0">
-        <v>321.0</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s" s="0">
-        <v>27</v>
-      </c>
-      <c r="B13" t="n" s="0">
-        <v>13.0</v>
-      </c>
-      <c r="C13" t="n" s="0">
         <v>542.0</v>
       </c>
     </row>

</xml_diff>